<commit_message>
Added option to skiprows while reading data file
</commit_message>
<xml_diff>
--- a/Data/BLscientist.xlsx
+++ b/Data/BLscientist.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,9 +21,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
-    <t>Badge No</t>
-  </si>
-  <si>
     <t>First Name</t>
   </si>
   <si>
@@ -76,6 +73,9 @@
   </si>
   <si>
     <t>Chen</t>
+  </si>
+  <si>
+    <t>Badge</t>
   </si>
 </sst>
 </file>
@@ -95,11 +95,13 @@
       <sz val="9"/>
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -466,90 +468,88 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="3" width="9.140625" style="4"/>
+    <col min="1" max="3" width="9.15625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="2" t="s">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="B3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="C3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="3" t="s">
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="B4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="C4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="3" t="s">
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="B5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="C5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="4">
         <v>85116</v>
       </c>
       <c r="B6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="4">
         <v>88772</v>
       </c>
       <c r="B7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>17</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>